<commit_message>
updating with scripts, figs, and data
</commit_message>
<xml_diff>
--- a/Data/FinnTumblingData.xlsx
+++ b/Data/FinnTumblingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wwu2-my.sharepoint.com/personal/pinkeb_wwu_edu/Documents/Thesis/ThesisCode/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C303B7EE-9BB2-9E45-858B-A480CD38741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD9AF889-A193-3E4A-9CDB-960CD5B9192F}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{C303B7EE-9BB2-9E45-858B-A480CD38741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E292137-6C40-874F-90A9-A52FA3E5C531}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="4" xr2:uid="{024021D0-AC20-4941-9B91-A8601D7B626B}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="160">
   <si>
     <t>Mass (g)</t>
   </si>
@@ -538,12 +538,24 @@
   </si>
   <si>
     <t>Abrasion Avg</t>
+  </si>
+  <si>
+    <t>Abr Error</t>
+  </si>
+  <si>
+    <t>Min Abrasion</t>
+  </si>
+  <si>
+    <t>Max Abrasion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -607,15 +619,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -623,15 +632,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,706 +1001,706 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="160" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>33</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="208" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>17</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>47</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="160" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>16</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>42</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="160" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>14</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>37</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="208" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>16</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>59.5</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="192" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>10</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="320" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>12</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="240" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>19</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>26</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="256" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>13</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>31</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="144" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>21</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>55</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>15</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>41.5</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>15</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>54</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>13</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>31</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="208" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>14</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>40</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="208" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>11</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>18</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="208" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>10</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="192" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>11</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>53</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="304" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>12</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>59</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="256" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>10</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="160" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>18</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>44</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="160" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>15</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>59</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1715,20 +1724,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="5:24" x14ac:dyDescent="0.2">
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
     </row>
     <row r="4" spans="5:24" x14ac:dyDescent="0.2">
       <c r="E4" s="1" t="s">
@@ -2985,7 +2994,7 @@
       <c r="J35">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="L35" s="9" t="s">
+      <c r="L35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="M35">
@@ -3003,7 +3012,7 @@
       <c r="J36">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L36" s="9" t="s">
+      <c r="L36" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M36">
@@ -3015,13 +3024,13 @@
       <c r="H37">
         <v>3</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J37" s="10">
+      <c r="J37" s="8">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="L37" s="9" t="s">
+      <c r="L37" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M37">
@@ -3033,13 +3042,13 @@
       <c r="H38">
         <v>4</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="8">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="L38" s="9" t="s">
+      <c r="L38" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M38">
@@ -3057,10 +3066,10 @@
       <c r="J39">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="L39" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M39" s="10">
+      <c r="M39" s="8">
         <f>AVERAGE(J37:J38)</f>
         <v>4.4999999999999999E-4</v>
       </c>
@@ -3075,7 +3084,7 @@
       <c r="J40">
         <v>1E-3</v>
       </c>
-      <c r="L40" s="9" t="s">
+      <c r="L40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M40">
@@ -3180,50 +3189,50 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>2.4131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>2.5888</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>2.5554999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>2.5036</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>2.4575</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>2.2835000000000001</v>
       </c>
     </row>
@@ -3250,16 +3259,16 @@
       <c r="A1" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="F1" t="s">
@@ -3268,7 +3277,7 @@
       <c r="G1" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3276,154 +3285,154 @@
       <c r="A2">
         <v>2023</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>37</v>
       </c>
       <c r="F2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>2.4131</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2023</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C3" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>26</v>
       </c>
       <c r="F3">
         <v>4.5499999999999999E-2</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>2.2835000000000001</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2023</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>143</v>
       </c>
       <c r="C4" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>55</v>
       </c>
       <c r="F4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>2.4575</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2023</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>144</v>
       </c>
       <c r="C5" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>53</v>
       </c>
       <c r="F5">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>2.5036</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>59</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6">
         <v>4.4999999999999999E-4</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>2.5888</v>
       </c>
-      <c r="K6" s="7"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2023</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>145</v>
       </c>
       <c r="C7" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>59</v>
       </c>
       <c r="F7">
         <v>2E-3</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>2.5554999999999999</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3432,111 +3441,268 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9648DD5C-6272-734E-AB0B-CF6C9D60C39E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B1" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="H1" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="6">
+      <c r="C2" s="5">
         <v>37</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2413.1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(E2:F2)</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="H2">
+        <f>F2-G2</f>
+        <v>1.4999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>2283.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="5">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>2457.5</v>
+      </c>
+      <c r="E4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G7" si="0">AVERAGE(E4:F4)</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" ref="H4:H7" si="1">F4-G4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="5">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>2503.6</v>
+      </c>
+      <c r="E5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F5">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6">
-        <v>26</v>
-      </c>
-      <c r="C3">
-        <v>2283.5</v>
-      </c>
-      <c r="D3">
-        <v>4.5499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="6">
-        <v>55</v>
-      </c>
-      <c r="C4">
-        <v>2457.5</v>
-      </c>
-      <c r="D4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="6">
-        <v>53</v>
-      </c>
-      <c r="C5">
-        <v>2503.6</v>
-      </c>
-      <c r="D5">
+      <c r="G5">
+        <f t="shared" si="0"/>
         <v>5.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.5000000000000005E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="6">
+      <c r="C6" s="5">
         <v>59</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2588.8000000000002</v>
       </c>
-      <c r="D6" s="11">
-        <v>4.4999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="E6">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F6">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H6">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="6">
+      <c r="C7" s="5">
         <v>59</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2555.5</v>
       </c>
-      <c r="D7">
+      <c r="E7">
+        <v>1E-3</v>
+      </c>
+      <c r="F7">
         <v>2E-3</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1.5E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>